<commit_message>
24-Feb-2017_1707- commiting fluent wait, SL workflow and Child-SL and Child-OB and OB Suite.xls(change in end date- without tested)
</commit_message>
<xml_diff>
--- a/src/test/resources/com/sirion/xls/Child Obligation Suite.xlsx
+++ b/src/test/resources/com/sirion/xls/Child Obligation Suite.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="165" windowWidth="14805" windowHeight="7950"/>
+    <workbookView xWindow="240" yWindow="165" windowWidth="14805" windowHeight="7950" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Test Cases" sheetId="1" r:id="rId1"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="32">
   <si>
     <t>TCID</t>
   </si>
@@ -36,9 +36,6 @@
     <t>Error</t>
   </si>
   <si>
-    <t>N</t>
-  </si>
-  <si>
     <t>ChildDNOUpdate</t>
   </si>
   <si>
@@ -84,40 +81,44 @@
     <t>Archive</t>
   </si>
   <si>
+    <t>WFTask3</t>
+  </si>
+  <si>
+    <t>Approve</t>
+  </si>
+  <si>
+    <t>WFTask4</t>
+  </si>
+  <si>
+    <t>Delete</t>
+  </si>
+  <si>
+    <t>OnHold</t>
+  </si>
+  <si>
+    <t>Resubmit</t>
+  </si>
+  <si>
+    <t>COB01024</t>
+  </si>
+  <si>
+    <t>PASS</t>
+  </si>
+  <si>
+    <t>FAIL</t>
+  </si>
+  <si>
+    <t>Reject</t>
+  </si>
+  <si>
     <t>Submit</t>
-  </si>
-  <si>
-    <t>WFTask3</t>
-  </si>
-  <si>
-    <t>Reject</t>
-  </si>
-  <si>
-    <t>Approve</t>
-  </si>
-  <si>
-    <t>WFTask4</t>
-  </si>
-  <si>
-    <t>Delete</t>
-  </si>
-  <si>
-    <t>OnHold</t>
-  </si>
-  <si>
-    <t>Resubmit</t>
-  </si>
-  <si>
-    <t>COB01024</t>
-  </si>
-  <si>
-    <t>PASS</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <numFmts count="0"/>
   <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -518,15 +519,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D3"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+    <sheetView showGridLines="0" workbookViewId="0">
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="2" width="36.85546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="23.7109375" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="7.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="2" bestFit="true" customWidth="true" width="36.85546875" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="23.7109375" collapsed="true"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="7.2578125" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
@@ -545,28 +546,30 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="D2" s="4"/>
+        <v>4</v>
+      </c>
+      <c r="D2" s="4" t="s">
+        <v>29</v>
+      </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C3" s="5" t="s">
         <v>4</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
     </row>
   </sheetData>
@@ -585,30 +588,30 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="9.7109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="3" width="14" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="16" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="27.5703125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="8.28515625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="7.28515625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="5.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="9.7109375" collapsed="true"/>
+    <col min="2" max="3" bestFit="true" customWidth="true" width="14.0" collapsed="true"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="16.0" collapsed="true"/>
+    <col min="5" max="5" bestFit="true" customWidth="true" width="27.5703125" collapsed="true"/>
+    <col min="6" max="6" bestFit="true" customWidth="true" width="8.28515625" collapsed="true"/>
+    <col min="7" max="7" bestFit="true" customWidth="true" width="7.2578125" collapsed="true"/>
+    <col min="8" max="8" bestFit="true" customWidth="true" width="5.28515625" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="B1" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="B1" s="3" t="s">
+      <c r="C1" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="C1" s="3" t="s">
+      <c r="D1" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="D1" s="3" t="s">
+      <c r="E1" s="3" t="s">
         <v>11</v>
-      </c>
-      <c r="E1" s="3" t="s">
-        <v>12</v>
       </c>
       <c r="F1" s="3" t="s">
         <v>2</v>
@@ -622,25 +625,25 @@
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="B2" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="B2" s="2" t="s">
+      <c r="C2" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="D2" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="C2" s="6" t="s">
-        <v>17</v>
-      </c>
-      <c r="D2" s="2" t="s">
+      <c r="E2" s="2" t="s">
         <v>15</v>
-      </c>
-      <c r="E2" s="2" t="s">
-        <v>16</v>
       </c>
       <c r="F2" s="2" t="s">
         <v>4</v>
       </c>
       <c r="G2" s="2" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="H2" s="2"/>
     </row>
@@ -653,43 +656,43 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L2"/>
   <sheetViews>
-    <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="K2" sqref="K2"/>
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="5" max="5" width="12.28515625" customWidth="1" collapsed="1"/>
-    <col min="11" max="11" width="7.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" customWidth="true" width="12.28515625" collapsed="true"/>
+    <col min="11" max="11" bestFit="true" customWidth="true" width="7.2578125" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="E1" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="B1" s="3" t="s">
+      <c r="F1" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="C1" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="D1" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="E1" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="F1" s="3" t="s">
+      <c r="G1" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="H1" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="G1" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="H1" s="3" t="s">
-        <v>26</v>
-      </c>
       <c r="I1" s="3" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="J1" s="3" t="s">
         <v>2</v>
@@ -703,28 +706,26 @@
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="B2" s="2" t="s">
         <v>4</v>
       </c>
       <c r="C2" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="F2" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="G2" s="2"/>
+      <c r="H2" s="2" t="s">
         <v>22</v>
-      </c>
-      <c r="D2" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="E2" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="F2" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="G2" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="H2" s="2" t="s">
-        <v>25</v>
       </c>
       <c r="I2" s="2" t="s">
         <v>4</v>
@@ -732,7 +733,9 @@
       <c r="J2" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="K2" s="2"/>
+      <c r="K2" s="2" t="s">
+        <v>29</v>
+      </c>
       <c r="L2" s="2"/>
     </row>
   </sheetData>

</xml_diff>